<commit_message>
Add Client class and different speed scenarios for LinkedList
The new Client class was implemented. We also added three different LinkedList speed scenarios using the Client class. In the LinkedList class, checks for `None` now use the 'is' operator. LinkedList's `remove` method now returns the removed data value.
</commit_message>
<xml_diff>
--- a/Table-of-Real-World-Speeds.xlsx
+++ b/Table-of-Real-World-Speeds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CEIS-295\CEIS295-Week2\Week 2 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1CA5C5-E530-4BDD-A62B-44159DCDA316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A4C2AD-1696-4B14-B0D0-2190F65A5544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="1425" windowWidth="21045" windowHeight="11295" xr2:uid="{6445DB60-6F86-45C9-B724-D766F58CE32D}"/>
+    <workbookView xWindow="28380" yWindow="1410" windowWidth="15855" windowHeight="10410" xr2:uid="{6445DB60-6F86-45C9-B724-D766F58CE32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Table of Real-World Speeds</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Add some records, display random records, remove random records</t>
+  </si>
+  <si>
+    <t>LINKED LISTS</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +120,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -131,55 +140,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -247,56 +207,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,257 +594,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DB1544-19F1-4E22-9949-635942135503}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="M5" s="13"/>
+      <c r="N5" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="7">
         <v>4.6319999999999998E-3</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16">
+      <c r="K7" s="7"/>
+      <c r="L7" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="M7" s="7"/>
+      <c r="N7" s="11">
+        <v>2.091E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="7">
         <v>2.6239710000000001</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16">
+      <c r="K8" s="7"/>
+      <c r="L8" s="7">
         <v>2.8312040000000001</v>
       </c>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="M8" s="7"/>
+      <c r="N8" s="11">
+        <v>1.5349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="7">
         <v>0.67555200000000004</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16">
+      <c r="K10" s="7"/>
+      <c r="L10" s="7">
         <v>1.2777999999999999E-2</v>
       </c>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="M10" s="7"/>
+      <c r="N10" s="11">
+        <v>0.48521799999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="17">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5">
         <v>1.6777930000000001</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="17">
+      <c r="K12" s="6"/>
+      <c r="L12" s="5">
         <v>1.4218580000000001</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="11">
+        <v>0.94074800000000003</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:N4"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="L12:M12"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A1:M4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>